<commit_message>
Arquivo com interface grafica feita e funcionando
</commit_message>
<xml_diff>
--- a/Vendas.xlsx
+++ b/Vendas.xlsx
@@ -877,7 +877,9 @@
       </c>
       <c r="Y2" s="3" t="n"/>
       <c r="Z2" s="3" t="n"/>
-      <c r="AA2" s="3" t="n"/>
+      <c r="AA2" s="3" t="n">
+        <v>32</v>
+      </c>
       <c r="AB2" s="3" t="n"/>
       <c r="AC2" s="3" t="n"/>
       <c r="AD2" s="3" t="n"/>
@@ -967,7 +969,9 @@
       </c>
       <c r="Y4" s="3" t="n"/>
       <c r="Z4" s="3" t="n"/>
-      <c r="AA4" s="3" t="n"/>
+      <c r="AA4" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="AB4" s="3" t="n"/>
       <c r="AC4" s="3" t="n"/>
       <c r="AD4" s="3" t="n"/>
@@ -1013,7 +1017,9 @@
       </c>
       <c r="Y5" s="3" t="n"/>
       <c r="Z5" s="3" t="n"/>
-      <c r="AA5" s="3" t="n"/>
+      <c r="AA5" s="3" t="n">
+        <v>63</v>
+      </c>
       <c r="AB5" s="3" t="n"/>
       <c r="AC5" s="3" t="n"/>
       <c r="AD5" s="3" t="n"/>
@@ -1059,7 +1065,9 @@
       </c>
       <c r="Y6" s="3" t="n"/>
       <c r="Z6" s="3" t="n"/>
-      <c r="AA6" s="3" t="n"/>
+      <c r="AA6" s="3" t="n">
+        <v>27</v>
+      </c>
       <c r="AB6" s="3" t="n"/>
       <c r="AC6" s="3" t="n"/>
       <c r="AD6" s="3" t="n"/>
@@ -1105,7 +1113,9 @@
       </c>
       <c r="Y7" s="3" t="n"/>
       <c r="Z7" s="3" t="n"/>
-      <c r="AA7" s="3" t="n"/>
+      <c r="AA7" s="3" t="n">
+        <v>52</v>
+      </c>
       <c r="AB7" s="3" t="n"/>
       <c r="AC7" s="3" t="n"/>
       <c r="AD7" s="3" t="n"/>
@@ -1283,7 +1293,9 @@
       </c>
       <c r="Y11" s="3" t="n"/>
       <c r="Z11" s="3" t="n"/>
-      <c r="AA11" s="3" t="n"/>
+      <c r="AA11" s="3" t="n">
+        <v>27</v>
+      </c>
       <c r="AB11" s="3" t="n"/>
       <c r="AC11" s="3" t="n"/>
       <c r="AD11" s="3" t="n"/>
@@ -1329,7 +1341,9 @@
       </c>
       <c r="Y12" s="3" t="n"/>
       <c r="Z12" s="3" t="n"/>
-      <c r="AA12" s="3" t="n"/>
+      <c r="AA12" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="AB12" s="3" t="n"/>
       <c r="AC12" s="3" t="n"/>
       <c r="AD12" s="3" t="n"/>
@@ -1375,7 +1389,9 @@
       </c>
       <c r="Y13" s="3" t="n"/>
       <c r="Z13" s="3" t="n"/>
-      <c r="AA13" s="3" t="n"/>
+      <c r="AA13" s="3" t="n">
+        <v>60</v>
+      </c>
       <c r="AB13" s="3" t="n"/>
       <c r="AC13" s="3" t="n"/>
       <c r="AD13" s="3" t="n"/>

</xml_diff>

<commit_message>
Aplicação com o arquivo executavel .exe
A aplicação agr roda um arquivo executavel
</commit_message>
<xml_diff>
--- a/Vendas.xlsx
+++ b/Vendas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5115" yWindow="3000" windowWidth="15375" windowHeight="7995" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
@@ -102,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -121,10 +121,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -405,7 +408,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -447,19 +450,19 @@
       <c r="A2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>Banana</t>
         </is>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="8" t="n">
         <v>74</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <f>Sheet1!AH2</f>
         <v/>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <f>C2-D2</f>
         <v/>
       </c>
@@ -468,19 +471,19 @@
       <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="8" t="inlineStr">
         <is>
           <t>Maça</t>
         </is>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>69</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <f>Sheet1!AH3</f>
         <v/>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <f>C3-D3</f>
         <v/>
       </c>
@@ -489,19 +492,19 @@
       <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>Melancia</t>
         </is>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="8" t="n">
         <v>33</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <f>Sheet1!AH4</f>
         <v/>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <f>C4-D4</f>
         <v/>
       </c>
@@ -510,19 +513,19 @@
       <c r="A5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>Uva</t>
         </is>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="8" t="n">
         <v>91</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <f>Sheet1!AH5</f>
         <v/>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <f>C5-D5</f>
         <v/>
       </c>
@@ -531,19 +534,19 @@
       <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>Mexirica</t>
         </is>
       </c>
-      <c r="C6" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C6" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="D6" s="8">
         <f>Sheet1!AH6</f>
         <v/>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <f>C6-D6</f>
         <v/>
       </c>
@@ -552,124 +555,124 @@
       <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>Cereja</t>
         </is>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="8" t="n">
         <v>72</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f>Sheet1!AH7</f>
         <v/>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <f>C7-D7</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Mamão</t>
         </is>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="8" t="n">
         <v>51</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f>Sheet1!AH8</f>
         <v/>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f>C8-D8</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="n">
+      <c r="A9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Melão</t>
         </is>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <f>Sheet1!AH9</f>
         <v/>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f>C9-D9</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="n">
+      <c r="A10" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="8" t="inlineStr">
         <is>
           <t>Abacate</t>
         </is>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="8" t="n">
         <v>48</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <f>Sheet1!AH10</f>
         <v/>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <f>C10-D10</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>Açai</t>
         </is>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="8" t="n">
         <v>83</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <f>Sheet1!AH11</f>
         <v/>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <f>C11-D11</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="n">
+      <c r="A12" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>Cacau</t>
         </is>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <f>Sheet1!AH12</f>
         <v/>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <f>C12-D12</f>
         <v/>
       </c>
@@ -686,11 +689,11 @@
       <c r="C13" s="4" t="n">
         <v>210</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f>Sheet1!AH13</f>
         <v/>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <f>C13-D13</f>
         <v/>
       </c>
@@ -710,7 +713,7 @@
   <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:W13"/>
+      <selection activeCell="AB13" sqref="AB2:AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -872,15 +875,13 @@
       <c r="U2" s="3" t="n"/>
       <c r="V2" s="3" t="n"/>
       <c r="W2" s="3" t="n"/>
-      <c r="X2" s="3" t="n">
-        <v>32</v>
-      </c>
+      <c r="X2" s="3" t="n"/>
       <c r="Y2" s="3" t="n"/>
       <c r="Z2" s="3" t="n"/>
-      <c r="AA2" s="3" t="n">
+      <c r="AA2" s="3" t="n"/>
+      <c r="AB2" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="AB2" s="3" t="n"/>
       <c r="AC2" s="3" t="n"/>
       <c r="AD2" s="3" t="n"/>
       <c r="AE2" s="3" t="n"/>
@@ -964,15 +965,13 @@
       <c r="U4" s="3" t="n"/>
       <c r="V4" s="3" t="n"/>
       <c r="W4" s="3" t="n"/>
-      <c r="X4" s="3" t="n">
-        <v>12</v>
-      </c>
+      <c r="X4" s="3" t="n"/>
       <c r="Y4" s="3" t="n"/>
       <c r="Z4" s="3" t="n"/>
-      <c r="AA4" s="3" t="n">
+      <c r="AA4" s="3" t="n"/>
+      <c r="AB4" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AB4" s="3" t="n"/>
       <c r="AC4" s="3" t="n"/>
       <c r="AD4" s="3" t="n"/>
       <c r="AE4" s="3" t="n"/>
@@ -1012,15 +1011,13 @@
       <c r="U5" s="3" t="n"/>
       <c r="V5" s="3" t="n"/>
       <c r="W5" s="3" t="n"/>
-      <c r="X5" s="3" t="n">
-        <v>63</v>
-      </c>
+      <c r="X5" s="3" t="n"/>
       <c r="Y5" s="3" t="n"/>
       <c r="Z5" s="3" t="n"/>
-      <c r="AA5" s="3" t="n">
+      <c r="AA5" s="3" t="n"/>
+      <c r="AB5" s="3" t="n">
         <v>63</v>
       </c>
-      <c r="AB5" s="3" t="n"/>
       <c r="AC5" s="3" t="n"/>
       <c r="AD5" s="3" t="n"/>
       <c r="AE5" s="3" t="n"/>
@@ -1060,15 +1057,13 @@
       <c r="U6" s="3" t="n"/>
       <c r="V6" s="3" t="n"/>
       <c r="W6" s="3" t="n"/>
-      <c r="X6" s="3" t="n">
-        <v>27</v>
-      </c>
+      <c r="X6" s="3" t="n"/>
       <c r="Y6" s="3" t="n"/>
       <c r="Z6" s="3" t="n"/>
-      <c r="AA6" s="3" t="n">
+      <c r="AA6" s="3" t="n"/>
+      <c r="AB6" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AB6" s="3" t="n"/>
       <c r="AC6" s="3" t="n"/>
       <c r="AD6" s="3" t="n"/>
       <c r="AE6" s="3" t="n"/>
@@ -1108,15 +1103,13 @@
       <c r="U7" s="3" t="n"/>
       <c r="V7" s="3" t="n"/>
       <c r="W7" s="3" t="n"/>
-      <c r="X7" s="3" t="n">
-        <v>52</v>
-      </c>
+      <c r="X7" s="3" t="n"/>
       <c r="Y7" s="3" t="n"/>
       <c r="Z7" s="3" t="n"/>
-      <c r="AA7" s="3" t="n">
+      <c r="AA7" s="3" t="n"/>
+      <c r="AB7" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="AB7" s="3" t="n"/>
       <c r="AC7" s="3" t="n"/>
       <c r="AD7" s="3" t="n"/>
       <c r="AE7" s="3" t="n"/>
@@ -1204,7 +1197,9 @@
       <c r="Y9" s="3" t="n"/>
       <c r="Z9" s="3" t="n"/>
       <c r="AA9" s="3" t="n"/>
-      <c r="AB9" s="3" t="n"/>
+      <c r="AB9" s="3" t="n">
+        <v>23</v>
+      </c>
       <c r="AC9" s="3" t="n"/>
       <c r="AD9" s="3" t="n"/>
       <c r="AE9" s="3" t="n"/>
@@ -1288,15 +1283,13 @@
       <c r="U11" s="3" t="n"/>
       <c r="V11" s="3" t="n"/>
       <c r="W11" s="3" t="n"/>
-      <c r="X11" s="3" t="n">
-        <v>27</v>
-      </c>
+      <c r="X11" s="3" t="n"/>
       <c r="Y11" s="3" t="n"/>
       <c r="Z11" s="3" t="n"/>
-      <c r="AA11" s="3" t="n">
+      <c r="AA11" s="3" t="n"/>
+      <c r="AB11" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AB11" s="3" t="n"/>
       <c r="AC11" s="3" t="n"/>
       <c r="AD11" s="3" t="n"/>
       <c r="AE11" s="3" t="n"/>
@@ -1336,15 +1329,13 @@
       <c r="U12" s="3" t="n"/>
       <c r="V12" s="3" t="n"/>
       <c r="W12" s="3" t="n"/>
-      <c r="X12" s="3" t="n">
-        <v>12</v>
-      </c>
+      <c r="X12" s="3" t="n"/>
       <c r="Y12" s="3" t="n"/>
       <c r="Z12" s="3" t="n"/>
-      <c r="AA12" s="3" t="n">
+      <c r="AA12" s="3" t="n"/>
+      <c r="AB12" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AB12" s="3" t="n"/>
       <c r="AC12" s="3" t="n"/>
       <c r="AD12" s="3" t="n"/>
       <c r="AE12" s="3" t="n"/>
@@ -1384,15 +1375,13 @@
       <c r="U13" s="3" t="n"/>
       <c r="V13" s="3" t="n"/>
       <c r="W13" s="3" t="n"/>
-      <c r="X13" s="3" t="n">
-        <v>60</v>
-      </c>
+      <c r="X13" s="3" t="n"/>
       <c r="Y13" s="3" t="n"/>
       <c r="Z13" s="3" t="n"/>
-      <c r="AA13" s="3" t="n">
+      <c r="AA13" s="3" t="n"/>
+      <c r="AB13" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="AB13" s="3" t="n"/>
       <c r="AC13" s="3" t="n"/>
       <c r="AD13" s="3" t="n"/>
       <c r="AE13" s="3" t="n"/>

</xml_diff>